<commit_message>
cleanning the backend code for weap and leap module
</commit_message>
<xml_diff>
--- a/Step_Control_Test/Test_Schedule_WEAP_LEAP_Time_Step_Control.xlsx
+++ b/Step_Control_Test/Test_Schedule_WEAP_LEAP_Time_Step_Control.xlsx
@@ -27,9 +27,6 @@
     <t>Method</t>
   </si>
   <si>
-    <t xml:space="preserve">Status </t>
-  </si>
-  <si>
     <t>Conclusion</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
   </si>
   <si>
     <t>Last Date Updated</t>
-  </si>
-  <si>
-    <t>Finished</t>
   </si>
   <si>
     <t>API:
@@ -86,61 +80,6 @@
 LEAP.BaseYear
 LEAP.FirstScenarioYear
 LEAP.EndYear</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This method requires the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>assumption</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> that WEAP and LEAp outputs have minimum or NO influence (feed back) to statistical model.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">This is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NOT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> a valid method.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -168,18 +107,36 @@
     </r>
   </si>
   <si>
+    <t>This method only allows WEAP and LEAP 
+to run from beginning year to a specified 
+year and does NOT give enough flexibility to let WEAP and LEAP to run on yearly basis.</t>
+  </si>
+  <si>
+    <t>Controlling through WEAP and LEAP software time step setting panel</t>
+  </si>
+  <si>
+    <t>There is no software built-in function to 
+run WEAP and LEAP by yearly steps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Status </t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">This is </t>
+      <t xml:space="preserve">This method requires the </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color theme="4" tint="-0.249977111117893"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>NOT</t>
+      <t>assumption</t>
     </r>
     <r>
       <rPr>
@@ -189,23 +146,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> a valid method.</t>
+      <t xml:space="preserve"> that WEAP and LEAP outputs have minimum or NO influence (feed back) to statistical model.</t>
     </r>
   </si>
   <si>
-    <t>This method only allows WEAP and LEAP 
-to run from beginning year to a specified 
-year and does NOT give enough flexibility to let WEAP and LEAP to run on yearly basis.</t>
-  </si>
-  <si>
-    <t>Controlling through WEAP and LEAP software time step setting panel</t>
-  </si>
-  <si>
-    <t>There is no software built-in function to 
-run WEAP and LEAP by yearly steps.</t>
-  </si>
-  <si>
-    <t>This is a valid way to control WEAP and LEAP time step at hightime cost for development.</t>
+    <t>This method only allows WEAP and LEAP to run over the full time span.</t>
+  </si>
+  <si>
+    <t>This method only controls the last time step.</t>
+  </si>
+  <si>
+    <t>This is a valid way to control WEAP and LEAP to run by yearly time step at high cost of time and labor for the development.</t>
   </si>
 </sst>
 </file>
@@ -389,22 +340,61 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -412,9 +402,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -422,59 +409,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,7 +710,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+      <selection activeCell="A12" sqref="A12:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +721,7 @@
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.42578125" customWidth="1"/>
     <col min="6" max="6" width="36.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -782,222 +733,204 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="B2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="9">
+        <v>43724</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="9">
+        <v>43724</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="23">
-        <v>43724</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="D7" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="23">
-        <v>43724</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="29"/>
-    </row>
-    <row r="6" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="28"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="30">
+      <c r="G7" s="12">
         <v>43737</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="31"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="31"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="31"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="13"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
-      <c r="G11" s="32"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="33"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>16</v>
+      <c r="C13" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="D13" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="30">
+      <c r="F13" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="12">
         <v>43738</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="31"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="16"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="26"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="32"/>
+      <c r="G15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="D13:D15"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
@@ -1008,6 +941,24 @@
     <mergeCell ref="F4:F6"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="F7:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>